<commit_message>
Cập nhật lại file thiết kế đến 12:00 221210
</commit_message>
<xml_diff>
--- a/root/common/doc/er図/テーブル定義書_BACSTEAM.xlsx
+++ b/root/common/doc/er図/テーブル定義書_BACSTEAM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="テーブル定義書" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="119">
   <si>
     <t xml:space="preserve">論理名</t>
   </si>
@@ -452,6 +452,12 @@
   <si>
     <t xml:space="preserve">https://www.navitime.co.jp/bus/company/00001054/</t>
   </si>
+  <si>
+    <t xml:space="preserve">biglobe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www5e.biglobe.ne.jp/~iwate/vehicle/extra/primer/basic/number_plate.html</t>
+  </si>
 </sst>
 </file>
 
@@ -460,7 +466,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -510,6 +516,12 @@
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -643,7 +655,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -744,76 +756,24 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -899,9 +859,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>41</xdr:col>
-      <xdr:colOff>181440</xdr:colOff>
+      <xdr:colOff>181080</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>3996720</xdr:rowOff>
+      <xdr:rowOff>3996360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -915,7 +875,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="43920" y="0"/>
-          <a:ext cx="12140280" cy="4172040"/>
+          <a:ext cx="12139920" cy="4171680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -937,7 +897,7 @@
   </sheetPr>
   <dimension ref="A1:AP1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="AL66" activeCellId="0" sqref="AL66"/>
     </sheetView>
   </sheetViews>
@@ -3105,223 +3065,223 @@
       <c r="AO47" s="9"/>
       <c r="AP47" s="8"/>
     </row>
-    <row r="48" s="31" customFormat="true" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="10"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="26" t="n">
+      <c r="B48" s="11"/>
+      <c r="C48" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="D48" s="27" t="s">
+      <c r="D48" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="E48" s="27"/>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
-      <c r="H48" s="27"/>
-      <c r="I48" s="28" t="s">
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="J48" s="28"/>
-      <c r="K48" s="28"/>
-      <c r="L48" s="28"/>
-      <c r="M48" s="28"/>
-      <c r="N48" s="28"/>
-      <c r="O48" s="28"/>
-      <c r="P48" s="28"/>
-      <c r="Q48" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="R48" s="29"/>
-      <c r="S48" s="28" t="s">
+      <c r="J48" s="14"/>
+      <c r="K48" s="14"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="14"/>
+      <c r="N48" s="14"/>
+      <c r="O48" s="14"/>
+      <c r="P48" s="14"/>
+      <c r="Q48" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="R48" s="15"/>
+      <c r="S48" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="T48" s="28"/>
-      <c r="U48" s="28"/>
-      <c r="V48" s="28"/>
-      <c r="W48" s="28"/>
-      <c r="X48" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y48" s="29"/>
-      <c r="Z48" s="29"/>
-      <c r="AA48" s="29"/>
-      <c r="AB48" s="25"/>
-      <c r="AC48" s="30"/>
-      <c r="AD48" s="30"/>
-      <c r="AE48" s="30"/>
-      <c r="AF48" s="30"/>
-      <c r="AG48" s="30"/>
-      <c r="AH48" s="30"/>
-      <c r="AI48" s="30"/>
-      <c r="AJ48" s="30"/>
-      <c r="AK48" s="30"/>
-      <c r="AL48" s="30"/>
-      <c r="AM48" s="30"/>
-      <c r="AN48" s="30"/>
-      <c r="AO48" s="30"/>
-      <c r="AP48" s="26"/>
-    </row>
-    <row r="49" s="31" customFormat="true" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="T48" s="14"/>
+      <c r="U48" s="14"/>
+      <c r="V48" s="14"/>
+      <c r="W48" s="14"/>
+      <c r="X48" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y48" s="15"/>
+      <c r="Z48" s="15"/>
+      <c r="AA48" s="15"/>
+      <c r="AB48" s="11"/>
+      <c r="AC48" s="16"/>
+      <c r="AD48" s="16"/>
+      <c r="AE48" s="16"/>
+      <c r="AF48" s="16"/>
+      <c r="AG48" s="16"/>
+      <c r="AH48" s="16"/>
+      <c r="AI48" s="16"/>
+      <c r="AJ48" s="16"/>
+      <c r="AK48" s="16"/>
+      <c r="AL48" s="16"/>
+      <c r="AM48" s="16"/>
+      <c r="AN48" s="16"/>
+      <c r="AO48" s="16"/>
+      <c r="AP48" s="12"/>
+    </row>
+    <row r="49" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="10"/>
-      <c r="B49" s="32"/>
-      <c r="C49" s="33" t="n">
+      <c r="B49" s="17"/>
+      <c r="C49" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="D49" s="34" t="s">
+      <c r="D49" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E49" s="35"/>
-      <c r="F49" s="35"/>
-      <c r="G49" s="35"/>
-      <c r="H49" s="33"/>
-      <c r="I49" s="28" t="s">
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="J49" s="28"/>
-      <c r="K49" s="28"/>
-      <c r="L49" s="28"/>
-      <c r="M49" s="28"/>
-      <c r="N49" s="28"/>
-      <c r="O49" s="28"/>
-      <c r="P49" s="28"/>
-      <c r="Q49" s="29"/>
-      <c r="R49" s="29"/>
-      <c r="S49" s="28" t="s">
+      <c r="J49" s="14"/>
+      <c r="K49" s="14"/>
+      <c r="L49" s="14"/>
+      <c r="M49" s="14"/>
+      <c r="N49" s="14"/>
+      <c r="O49" s="14"/>
+      <c r="P49" s="14"/>
+      <c r="Q49" s="15"/>
+      <c r="R49" s="15"/>
+      <c r="S49" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="T49" s="28"/>
-      <c r="U49" s="28"/>
-      <c r="V49" s="28"/>
-      <c r="W49" s="28"/>
-      <c r="X49" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y49" s="29"/>
-      <c r="Z49" s="29"/>
-      <c r="AA49" s="29"/>
-      <c r="AB49" s="32"/>
-      <c r="AC49" s="35"/>
-      <c r="AD49" s="35"/>
-      <c r="AE49" s="35"/>
-      <c r="AF49" s="35"/>
-      <c r="AG49" s="35"/>
-      <c r="AH49" s="35"/>
-      <c r="AI49" s="35"/>
-      <c r="AJ49" s="35"/>
-      <c r="AK49" s="35"/>
-      <c r="AL49" s="35"/>
-      <c r="AM49" s="35"/>
-      <c r="AN49" s="35"/>
-      <c r="AO49" s="35"/>
-      <c r="AP49" s="33"/>
-    </row>
-    <row r="50" s="31" customFormat="true" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="T49" s="14"/>
+      <c r="U49" s="14"/>
+      <c r="V49" s="14"/>
+      <c r="W49" s="14"/>
+      <c r="X49" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y49" s="15"/>
+      <c r="Z49" s="15"/>
+      <c r="AA49" s="15"/>
+      <c r="AB49" s="17"/>
+      <c r="AC49" s="21"/>
+      <c r="AD49" s="21"/>
+      <c r="AE49" s="21"/>
+      <c r="AF49" s="21"/>
+      <c r="AG49" s="21"/>
+      <c r="AH49" s="21"/>
+      <c r="AI49" s="21"/>
+      <c r="AJ49" s="21"/>
+      <c r="AK49" s="21"/>
+      <c r="AL49" s="21"/>
+      <c r="AM49" s="21"/>
+      <c r="AN49" s="21"/>
+      <c r="AO49" s="21"/>
+      <c r="AP49" s="18"/>
+    </row>
+    <row r="50" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="10"/>
-      <c r="B50" s="32"/>
-      <c r="C50" s="33" t="n">
+      <c r="B50" s="17"/>
+      <c r="C50" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="D50" s="34" t="s">
+      <c r="D50" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="E50" s="35"/>
-      <c r="F50" s="35"/>
-      <c r="G50" s="35"/>
-      <c r="H50" s="33"/>
-      <c r="I50" s="32" t="s">
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="J50" s="35"/>
-      <c r="K50" s="35"/>
-      <c r="L50" s="35"/>
-      <c r="M50" s="35"/>
-      <c r="N50" s="35"/>
-      <c r="O50" s="35"/>
-      <c r="P50" s="33"/>
-      <c r="Q50" s="36"/>
-      <c r="R50" s="37"/>
-      <c r="S50" s="38" t="s">
+      <c r="J50" s="21"/>
+      <c r="K50" s="21"/>
+      <c r="L50" s="21"/>
+      <c r="M50" s="21"/>
+      <c r="N50" s="21"/>
+      <c r="O50" s="21"/>
+      <c r="P50" s="18"/>
+      <c r="Q50" s="22"/>
+      <c r="R50" s="23"/>
+      <c r="S50" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="T50" s="38"/>
-      <c r="U50" s="38"/>
-      <c r="V50" s="38"/>
-      <c r="W50" s="38"/>
-      <c r="X50" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y50" s="29"/>
-      <c r="Z50" s="29"/>
-      <c r="AA50" s="29"/>
-      <c r="AB50" s="32"/>
-      <c r="AC50" s="35"/>
-      <c r="AD50" s="35"/>
-      <c r="AE50" s="35"/>
-      <c r="AF50" s="35"/>
-      <c r="AG50" s="35"/>
-      <c r="AH50" s="35"/>
-      <c r="AI50" s="35"/>
-      <c r="AJ50" s="35"/>
-      <c r="AK50" s="35"/>
-      <c r="AL50" s="35"/>
-      <c r="AM50" s="35"/>
-      <c r="AN50" s="35"/>
-      <c r="AO50" s="35"/>
-      <c r="AP50" s="33"/>
-    </row>
-    <row r="51" s="31" customFormat="true" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="T50" s="20"/>
+      <c r="U50" s="20"/>
+      <c r="V50" s="20"/>
+      <c r="W50" s="20"/>
+      <c r="X50" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y50" s="15"/>
+      <c r="Z50" s="15"/>
+      <c r="AA50" s="15"/>
+      <c r="AB50" s="17"/>
+      <c r="AC50" s="21"/>
+      <c r="AD50" s="21"/>
+      <c r="AE50" s="21"/>
+      <c r="AF50" s="21"/>
+      <c r="AG50" s="21"/>
+      <c r="AH50" s="21"/>
+      <c r="AI50" s="21"/>
+      <c r="AJ50" s="21"/>
+      <c r="AK50" s="21"/>
+      <c r="AL50" s="21"/>
+      <c r="AM50" s="21"/>
+      <c r="AN50" s="21"/>
+      <c r="AO50" s="21"/>
+      <c r="AP50" s="18"/>
+    </row>
+    <row r="51" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="10"/>
-      <c r="B51" s="32"/>
-      <c r="C51" s="33" t="n">
+      <c r="B51" s="17"/>
+      <c r="C51" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="D51" s="34" t="s">
+      <c r="D51" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="E51" s="35"/>
-      <c r="F51" s="35"/>
-      <c r="G51" s="35"/>
-      <c r="H51" s="33"/>
-      <c r="I51" s="28" t="s">
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
+      <c r="H51" s="18"/>
+      <c r="I51" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="J51" s="28"/>
-      <c r="K51" s="28"/>
-      <c r="L51" s="28"/>
-      <c r="M51" s="28"/>
-      <c r="N51" s="28"/>
-      <c r="O51" s="28"/>
-      <c r="P51" s="28"/>
-      <c r="Q51" s="36"/>
-      <c r="R51" s="37"/>
-      <c r="S51" s="28" t="s">
+      <c r="J51" s="14"/>
+      <c r="K51" s="14"/>
+      <c r="L51" s="14"/>
+      <c r="M51" s="14"/>
+      <c r="N51" s="14"/>
+      <c r="O51" s="14"/>
+      <c r="P51" s="14"/>
+      <c r="Q51" s="22"/>
+      <c r="R51" s="23"/>
+      <c r="S51" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="T51" s="28"/>
-      <c r="U51" s="28"/>
-      <c r="V51" s="28"/>
-      <c r="W51" s="28"/>
-      <c r="X51" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y51" s="29"/>
-      <c r="Z51" s="29"/>
-      <c r="AA51" s="29"/>
-      <c r="AB51" s="32"/>
-      <c r="AC51" s="35"/>
-      <c r="AD51" s="35"/>
-      <c r="AE51" s="35"/>
-      <c r="AF51" s="35"/>
-      <c r="AG51" s="35"/>
-      <c r="AH51" s="35"/>
-      <c r="AI51" s="35"/>
-      <c r="AJ51" s="35"/>
-      <c r="AK51" s="35"/>
-      <c r="AL51" s="35"/>
-      <c r="AM51" s="35"/>
-      <c r="AN51" s="35"/>
-      <c r="AO51" s="35"/>
-      <c r="AP51" s="33"/>
+      <c r="T51" s="14"/>
+      <c r="U51" s="14"/>
+      <c r="V51" s="14"/>
+      <c r="W51" s="14"/>
+      <c r="X51" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y51" s="15"/>
+      <c r="Z51" s="15"/>
+      <c r="AA51" s="15"/>
+      <c r="AB51" s="17"/>
+      <c r="AC51" s="21"/>
+      <c r="AD51" s="21"/>
+      <c r="AE51" s="21"/>
+      <c r="AF51" s="21"/>
+      <c r="AG51" s="21"/>
+      <c r="AH51" s="21"/>
+      <c r="AI51" s="21"/>
+      <c r="AJ51" s="21"/>
+      <c r="AK51" s="21"/>
+      <c r="AL51" s="21"/>
+      <c r="AM51" s="21"/>
+      <c r="AN51" s="21"/>
+      <c r="AO51" s="21"/>
+      <c r="AP51" s="18"/>
     </row>
     <row r="53" customFormat="false" ht="17.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="4" t="s">
@@ -3420,13 +3380,13 @@
       <c r="C55" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="D55" s="39" t="s">
+      <c r="D55" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="E55" s="39"/>
-      <c r="F55" s="39"/>
-      <c r="G55" s="39"/>
-      <c r="H55" s="39"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="25"/>
+      <c r="G55" s="25"/>
+      <c r="H55" s="25"/>
       <c r="I55" s="14" t="s">
         <v>49</v>
       </c>
@@ -3476,13 +3436,13 @@
       <c r="C56" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="D56" s="39" t="s">
+      <c r="D56" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="E56" s="39"/>
-      <c r="F56" s="39"/>
-      <c r="G56" s="39"/>
-      <c r="H56" s="39"/>
+      <c r="E56" s="25"/>
+      <c r="F56" s="25"/>
+      <c r="G56" s="25"/>
+      <c r="H56" s="25"/>
       <c r="I56" s="14" t="s">
         <v>87</v>
       </c>
@@ -3534,13 +3494,13 @@
       <c r="C57" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="D57" s="39" t="s">
+      <c r="D57" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="E57" s="39"/>
-      <c r="F57" s="39"/>
-      <c r="G57" s="39"/>
-      <c r="H57" s="39"/>
+      <c r="E57" s="25"/>
+      <c r="F57" s="25"/>
+      <c r="G57" s="25"/>
+      <c r="H57" s="25"/>
       <c r="I57" s="14" t="s">
         <v>90</v>
       </c>
@@ -3592,13 +3552,13 @@
       <c r="C58" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="D58" s="39" t="s">
+      <c r="D58" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="E58" s="39"/>
-      <c r="F58" s="39"/>
-      <c r="G58" s="39"/>
-      <c r="H58" s="39"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="25"/>
+      <c r="H58" s="25"/>
       <c r="I58" s="14" t="s">
         <v>92</v>
       </c>
@@ -3646,13 +3606,13 @@
       <c r="C59" s="12" t="n">
         <v>5</v>
       </c>
-      <c r="D59" s="39" t="s">
+      <c r="D59" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="E59" s="39"/>
-      <c r="F59" s="39"/>
-      <c r="G59" s="39"/>
-      <c r="H59" s="39"/>
+      <c r="E59" s="25"/>
+      <c r="F59" s="25"/>
+      <c r="G59" s="25"/>
+      <c r="H59" s="25"/>
       <c r="I59" s="14" t="s">
         <v>10</v>
       </c>
@@ -3704,13 +3664,13 @@
       <c r="C60" s="18" t="n">
         <v>6</v>
       </c>
-      <c r="D60" s="39" t="s">
+      <c r="D60" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="E60" s="39"/>
-      <c r="F60" s="39"/>
-      <c r="G60" s="39"/>
-      <c r="H60" s="39"/>
+      <c r="E60" s="25"/>
+      <c r="F60" s="25"/>
+      <c r="G60" s="25"/>
+      <c r="H60" s="25"/>
       <c r="I60" s="14" t="s">
         <v>95</v>
       </c>
@@ -3758,13 +3718,13 @@
       <c r="C61" s="12" t="n">
         <v>7</v>
       </c>
-      <c r="D61" s="39" t="s">
+      <c r="D61" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="E61" s="39"/>
-      <c r="F61" s="39"/>
-      <c r="G61" s="39"/>
-      <c r="H61" s="39"/>
+      <c r="E61" s="25"/>
+      <c r="F61" s="25"/>
+      <c r="G61" s="25"/>
+      <c r="H61" s="25"/>
       <c r="I61" s="14" t="s">
         <v>98</v>
       </c>
@@ -3812,13 +3772,13 @@
       <c r="C62" s="12" t="n">
         <v>8</v>
       </c>
-      <c r="D62" s="39" t="s">
+      <c r="D62" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="E62" s="39"/>
-      <c r="F62" s="39"/>
-      <c r="G62" s="39"/>
-      <c r="H62" s="39"/>
+      <c r="E62" s="25"/>
+      <c r="F62" s="25"/>
+      <c r="G62" s="25"/>
+      <c r="H62" s="25"/>
       <c r="I62" s="14" t="s">
         <v>100</v>
       </c>
@@ -3866,13 +3826,13 @@
       <c r="C63" s="12" t="n">
         <v>9</v>
       </c>
-      <c r="D63" s="39" t="s">
+      <c r="D63" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="E63" s="39"/>
-      <c r="F63" s="39"/>
-      <c r="G63" s="39"/>
-      <c r="H63" s="39"/>
+      <c r="E63" s="25"/>
+      <c r="F63" s="25"/>
+      <c r="G63" s="25"/>
+      <c r="H63" s="25"/>
       <c r="I63" s="14" t="s">
         <v>102</v>
       </c>
@@ -4148,89 +4108,102 @@
   </sheetPr>
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="40" width="6.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="74.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="6.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="39.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="26.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="74.09"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="27" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="40" t="n">
+      <c r="A2" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="28" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="40" t="n">
+      <c r="A3" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="28" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="28" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="26" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
     <row r="7" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4258,6 +4231,7 @@
     <hyperlink ref="D3" r:id="rId2" display="https://nlftp.mlit.go.jp/ksj/index.html"/>
     <hyperlink ref="D4" r:id="rId3" display="https://nlftp.mlit.go.jp/ksj/index.html"/>
     <hyperlink ref="D5" r:id="rId4" display="https://www.navitime.co.jp/bus/company/00001054/"/>
+    <hyperlink ref="D6" r:id="rId5" display="http://www5e.biglobe.ne.jp/~iwate/vehicle/extra/primer/basic/number_plate.html"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>